<commit_message>
Added the excel files from 12-17-19 to the directory and saved the images produced by all of the excel files
</commit_message>
<xml_diff>
--- a/12-9-19-hand-high.xlsx
+++ b/12-9-19-hand-high.xlsx
@@ -1143,19 +1143,19 @@
         <v>0</v>
       </c>
       <c r="B2" t="n">
-        <v>0.03366189246075152</v>
+        <v>0.03366188641270224</v>
       </c>
       <c r="C2" t="n">
-        <v>0.9663381075392485</v>
+        <v>0.9663381135872977</v>
       </c>
       <c r="D2" t="n">
-        <v>0.1357758050153616</v>
+        <v>0.1357758067762702</v>
       </c>
       <c r="E2" t="n">
-        <v>0.1187168911211204</v>
+        <v>0.1187168926612073</v>
       </c>
       <c r="F2" t="n">
-        <v>1.000000000016642</v>
+        <v>1.000000012986078</v>
       </c>
     </row>
     <row r="3">
@@ -1163,19 +1163,19 @@
         <v>5</v>
       </c>
       <c r="B3" t="n">
-        <v>0.0735241705363408</v>
+        <v>0.07352416473845924</v>
       </c>
       <c r="C3" t="n">
-        <v>0.9264758294636593</v>
+        <v>0.9264758352615408</v>
       </c>
       <c r="D3" t="n">
-        <v>0.1866266578362586</v>
+        <v>0.186626660373423</v>
       </c>
       <c r="E3" t="n">
-        <v>0.182452343028513</v>
+        <v>0.1824523455095254</v>
       </c>
       <c r="F3" t="n">
-        <v>1.000000000016884</v>
+        <v>1.000000013612186</v>
       </c>
     </row>
     <row r="4">
@@ -1183,19 +1183,19 @@
         <v>10</v>
       </c>
       <c r="B4" t="n">
-        <v>0.1409473594136893</v>
+        <v>0.1409473545241</v>
       </c>
       <c r="C4" t="n">
-        <v>0.8590526405863107</v>
+        <v>0.8590526454759</v>
       </c>
       <c r="D4" t="n">
-        <v>0.24309785953877</v>
+        <v>0.2430978628492838</v>
       </c>
       <c r="E4" t="n">
-        <v>0.2489671303278719</v>
+        <v>0.2489671337193434</v>
       </c>
       <c r="F4" t="n">
-        <v>1.000000000016059</v>
+        <v>1.000000013635114</v>
       </c>
     </row>
     <row r="5">
@@ -1203,19 +1203,19 @@
         <v>15</v>
       </c>
       <c r="B5" t="n">
-        <v>0.2481579828521254</v>
+        <v>0.2481579751059969</v>
       </c>
       <c r="C5" t="n">
-        <v>0.7518420171478746</v>
+        <v>0.7518420248940031</v>
       </c>
       <c r="D5" t="n">
-        <v>0.2964457503639625</v>
+        <v>0.2964457594820074</v>
       </c>
       <c r="E5" t="n">
-        <v>0.3141584242026197</v>
+        <v>0.3141584338671355</v>
       </c>
       <c r="F5" t="n">
-        <v>1.000000000014873</v>
+        <v>1.000000030774854</v>
       </c>
     </row>
     <row r="6">
@@ -1223,19 +1223,19 @@
         <v>20</v>
       </c>
       <c r="B6" t="n">
-        <v>0.3998504380237913</v>
+        <v>0.3998504343801063</v>
       </c>
       <c r="C6" t="n">
-        <v>0.6001495619762087</v>
+        <v>0.6001495656198937</v>
       </c>
       <c r="D6" t="n">
-        <v>0.33498301764456</v>
+        <v>0.3349830298320584</v>
       </c>
       <c r="E6" t="n">
-        <v>0.357430333257818</v>
+        <v>0.3574303462641036</v>
       </c>
       <c r="F6" t="n">
-        <v>1.000000000014154</v>
+        <v>1.000000036399592</v>
       </c>
     </row>
     <row r="7">
@@ -1243,19 +1243,19 @@
         <v>25</v>
       </c>
       <c r="B7" t="n">
-        <v>0.6105546994995934</v>
+        <v>0.6105547035240795</v>
       </c>
       <c r="C7" t="n">
-        <v>0.3894453005004067</v>
+        <v>0.3894452964759205</v>
       </c>
       <c r="D7" t="n">
-        <v>0.3333915156784608</v>
+        <v>0.3333915278148021</v>
       </c>
       <c r="E7" t="n">
-        <v>0.355847939012225</v>
+        <v>0.3558479519681307</v>
       </c>
       <c r="F7" t="n">
-        <v>1.00000000001415</v>
+        <v>1.000000036419796</v>
       </c>
     </row>
     <row r="8">
@@ -1263,19 +1263,19 @@
         <v>30</v>
       </c>
       <c r="B8" t="n">
-        <v>0.7730355115875289</v>
+        <v>0.7730355194975116</v>
       </c>
       <c r="C8" t="n">
-        <v>0.2269644884124711</v>
+        <v>0.2269644805024884</v>
       </c>
       <c r="D8" t="n">
-        <v>0.28726277185175</v>
+        <v>0.2872627801739042</v>
       </c>
       <c r="E8" t="n">
-        <v>0.304847026109327</v>
+        <v>0.3048470349424793</v>
       </c>
       <c r="F8" t="n">
-        <v>1.00000000001503</v>
+        <v>1.000000028987476</v>
       </c>
     </row>
     <row r="9">
@@ -1283,19 +1283,19 @@
         <v>35</v>
       </c>
       <c r="B9" t="n">
-        <v>0.8725975814955733</v>
+        <v>0.8725975861993882</v>
       </c>
       <c r="C9" t="n">
-        <v>0.1274024185044267</v>
+        <v>0.1274024138006118</v>
       </c>
       <c r="D9" t="n">
-        <v>0.231338058840658</v>
+        <v>0.2313380617611586</v>
       </c>
       <c r="E9" t="n">
-        <v>0.2401119422344123</v>
+        <v>0.2401119452666387</v>
       </c>
       <c r="F9" t="n">
-        <v>1.000000000016192</v>
+        <v>1.000000012641499</v>
       </c>
     </row>
     <row r="10">
@@ -1303,19 +1303,19 @@
         <v>40</v>
       </c>
       <c r="B10" t="n">
-        <v>0.9392430537167098</v>
+        <v>0.9392430595250765</v>
       </c>
       <c r="C10" t="n">
-        <v>0.0607569462832902</v>
+        <v>0.06075694047492347</v>
       </c>
       <c r="D10" t="n">
-        <v>0.1738217010154074</v>
+        <v>0.173821703313953</v>
       </c>
       <c r="E10" t="n">
-        <v>0.1638644440569899</v>
+        <v>0.1638644462244244</v>
       </c>
       <c r="F10" t="n">
-        <v>1.000000000016753</v>
+        <v>1.000000013240702</v>
       </c>
     </row>
     <row r="11">
@@ -1323,19 +1323,19 @@
         <v>45</v>
       </c>
       <c r="B11" t="n">
-        <v>0.9713245280095515</v>
+        <v>0.9713245340057686</v>
       </c>
       <c r="C11" t="n">
-        <v>0.02867547199044845</v>
+        <v>0.02867546599423149</v>
       </c>
       <c r="D11" t="n">
-        <v>0.1317422856236969</v>
+        <v>0.1317422872997296</v>
       </c>
       <c r="E11" t="n">
-        <v>0.1024556464205609</v>
+        <v>0.1024556477243875</v>
       </c>
       <c r="F11" t="n">
-        <v>1.000000000016474</v>
+        <v>1.000000012738686</v>
       </c>
     </row>
     <row r="12">
@@ -1343,19 +1343,19 @@
         <v>50</v>
       </c>
       <c r="B12" t="n">
-        <v>0.9903352366505965</v>
+        <v>0.9903352503015272</v>
       </c>
       <c r="C12" t="n">
-        <v>0.009664763349403471</v>
+        <v>0.009664749698472697</v>
       </c>
       <c r="D12" t="n">
-        <v>0.09157059512682571</v>
+        <v>0.09157059767615071</v>
       </c>
       <c r="E12" t="n">
-        <v>0.0344409903238185</v>
+        <v>0.0344409912828303</v>
       </c>
       <c r="F12" t="n">
-        <v>1.000000000015126</v>
+        <v>1.000000027855146</v>
       </c>
     </row>
     <row r="13">
@@ -1363,19 +1363,19 @@
         <v>55</v>
       </c>
       <c r="B13" t="n">
-        <v>0.9963286252939227</v>
+        <v>0.9963286455769149</v>
       </c>
       <c r="C13" t="n">
-        <v>0.003671374706077313</v>
+        <v>0.003671354423085138</v>
       </c>
       <c r="D13" t="n">
-        <v>0.04751973983429064</v>
+        <v>0.04751974177623489</v>
       </c>
       <c r="E13" t="n">
-        <v>-0.03741350085748</v>
+        <v>-0.03741350238665968</v>
       </c>
       <c r="F13" t="n">
-        <v>1.000000000012973</v>
+        <v>1.000000040879063</v>
       </c>
     </row>
     <row r="14">
@@ -1383,19 +1383,19 @@
         <v>60</v>
       </c>
       <c r="B14" t="n">
-        <v>0.9797491416868456</v>
+        <v>0.9797491418838395</v>
       </c>
       <c r="C14" t="n">
-        <v>0.02025085831315449</v>
+        <v>0.02025085811616045</v>
       </c>
       <c r="D14" t="n">
-        <v>0.00516771583489042</v>
+        <v>0.005167715837012384</v>
       </c>
       <c r="E14" t="n">
-        <v>-0.1407624089348517</v>
+        <v>-0.1407624089932488</v>
       </c>
       <c r="F14" t="n">
-        <v>1.000000000010715</v>
+        <v>1.00000000042167</v>
       </c>
     </row>
     <row r="15">
@@ -1403,19 +1403,19 @@
         <v>65</v>
       </c>
       <c r="B15" t="n">
-        <v>0.8130426204002541</v>
+        <v>0.81304262030736</v>
       </c>
       <c r="C15" t="n">
-        <v>0.186957379599746</v>
+        <v>0.18695737969264</v>
       </c>
       <c r="D15" t="n">
-        <v>-0.05869549132504764</v>
+        <v>-0.05869549130762999</v>
       </c>
       <c r="E15" t="n">
-        <v>-0.3854337263731187</v>
+        <v>-0.3854337262534369</v>
       </c>
       <c r="F15" t="n">
-        <v>1.000000000629629</v>
+        <v>1.000000000324703</v>
       </c>
     </row>
     <row r="16">
@@ -1423,19 +1423,19 @@
         <v>70</v>
       </c>
       <c r="B16" t="n">
-        <v>0.1184442190448523</v>
+        <v>0.1184442191853978</v>
       </c>
       <c r="C16" t="n">
-        <v>0.8815557809551477</v>
+        <v>0.8815557808146022</v>
       </c>
       <c r="D16" t="n">
-        <v>-0.04242672489725154</v>
+        <v>-0.04242672488162371</v>
       </c>
       <c r="E16" t="n">
-        <v>-0.3203360101321032</v>
+        <v>-0.3203360100122593</v>
       </c>
       <c r="F16" t="n">
-        <v>1.000000000706309</v>
+        <v>1.000000000335592</v>
       </c>
     </row>
     <row r="17">
@@ -1443,19 +1443,19 @@
         <v>75</v>
       </c>
       <c r="B17" t="n">
-        <v>0.01202997216441065</v>
+        <v>0.01202997196045735</v>
       </c>
       <c r="C17" t="n">
-        <v>0.9879700278355894</v>
+        <v>0.9879700280395427</v>
       </c>
       <c r="D17" t="n">
-        <v>0.02029597066634108</v>
+        <v>0.02029597067482406</v>
       </c>
       <c r="E17" t="n">
-        <v>-0.1071136103133075</v>
+        <v>-0.1071136103585912</v>
       </c>
       <c r="F17" t="n">
-        <v>1.000000000011012</v>
+        <v>1.000000000429195</v>
       </c>
     </row>
     <row r="18">
@@ -1463,19 +1463,19 @@
         <v>80</v>
       </c>
       <c r="B18" t="n">
-        <v>0.00371064087037154</v>
+        <v>0.003710621116476576</v>
       </c>
       <c r="C18" t="n">
-        <v>0.9962893591296285</v>
+        <v>0.9962893788835234</v>
       </c>
       <c r="D18" t="n">
-        <v>0.06054730181381467</v>
+        <v>0.06054730422378987</v>
       </c>
       <c r="E18" t="n">
-        <v>-0.005558440822216728</v>
+        <v>-0.005558441043495448</v>
       </c>
       <c r="F18" t="n">
-        <v>1.000000000013209</v>
+        <v>1.000000039816391</v>
       </c>
     </row>
     <row r="19">
@@ -1483,19 +1483,19 @@
         <v>85</v>
       </c>
       <c r="B19" t="n">
-        <v>0.01462419782405366</v>
+        <v>0.01462418593750031</v>
       </c>
       <c r="C19" t="n">
-        <v>0.9853758021759463</v>
+        <v>0.9853758140624997</v>
       </c>
       <c r="D19" t="n">
-        <v>0.1006007130007166</v>
+        <v>0.1006007154643659</v>
       </c>
       <c r="E19" t="n">
-        <v>0.06549677254255873</v>
+        <v>0.06549677414685051</v>
       </c>
       <c r="F19" t="n">
-        <v>1.000000000015375</v>
+        <v>1.00000002450484</v>
       </c>
     </row>
     <row r="20">
@@ -1503,19 +1503,19 @@
         <v>90</v>
       </c>
       <c r="B20" t="n">
-        <v>0.03612809939371803</v>
+        <v>0.03612809330644667</v>
       </c>
       <c r="C20" t="n">
-        <v>0.9638719006062819</v>
+        <v>0.9638719066935533</v>
       </c>
       <c r="D20" t="n">
-        <v>0.1395918103316799</v>
+        <v>0.1395918121635073</v>
       </c>
       <c r="E20" t="n">
-        <v>0.1238425868778453</v>
+        <v>0.123842588503428</v>
       </c>
       <c r="F20" t="n">
-        <v>1.000000000016713</v>
+        <v>1.000000013139668</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added err_corr2.py which is a file attempting the same thing as err_corr.py but using simpler syntax for cvxpy in order to determine if that's where the discrepancy between the polarimeter results and the code results came from.  Seems likely at this point
</commit_message>
<xml_diff>
--- a/12-9-19-hand-high.xlsx
+++ b/12-9-19-hand-high.xlsx
@@ -1143,19 +1143,19 @@
         <v>0</v>
       </c>
       <c r="B2" t="n">
-        <v>0.03366188641270224</v>
+        <v>0.03366188766086309</v>
       </c>
       <c r="C2" t="n">
-        <v>0.9663381135872977</v>
+        <v>0.9663381123391369</v>
       </c>
       <c r="D2" t="n">
-        <v>0.1357758067762702</v>
+        <v>0.1357758064128642</v>
       </c>
       <c r="E2" t="n">
-        <v>0.1187168926612073</v>
+        <v>0.1187168923434598</v>
       </c>
       <c r="F2" t="n">
-        <v>1.000000012986078</v>
+        <v>1.000000010309563</v>
       </c>
     </row>
     <row r="3">
@@ -1163,19 +1163,19 @@
         <v>5</v>
       </c>
       <c r="B3" t="n">
-        <v>0.07352416473845924</v>
+        <v>0.07352416749458512</v>
       </c>
       <c r="C3" t="n">
-        <v>0.9264758352615408</v>
+        <v>0.9264758325054149</v>
       </c>
       <c r="D3" t="n">
-        <v>0.186626660373423</v>
+        <v>0.1866266591673369</v>
       </c>
       <c r="E3" t="n">
-        <v>0.1824523455095254</v>
+        <v>0.182452344330416</v>
       </c>
       <c r="F3" t="n">
-        <v>1.000000013612186</v>
+        <v>1.000000007149625</v>
       </c>
     </row>
     <row r="4">
@@ -1183,19 +1183,19 @@
         <v>10</v>
       </c>
       <c r="B4" t="n">
-        <v>0.1409473545241</v>
+        <v>0.1409473534825794</v>
       </c>
       <c r="C4" t="n">
-        <v>0.8590526454759</v>
+        <v>0.8590526465174206</v>
       </c>
       <c r="D4" t="n">
-        <v>0.2430978628492838</v>
+        <v>0.243097863554449</v>
       </c>
       <c r="E4" t="n">
-        <v>0.2489671337193434</v>
+        <v>0.2489671344415339</v>
       </c>
       <c r="F4" t="n">
-        <v>1.000000013635114</v>
+        <v>1.00000001653586</v>
       </c>
     </row>
     <row r="5">
@@ -1203,19 +1203,19 @@
         <v>15</v>
       </c>
       <c r="B5" t="n">
-        <v>0.2481579751059969</v>
+        <v>0.2481579764058038</v>
       </c>
       <c r="C5" t="n">
-        <v>0.7518420248940031</v>
+        <v>0.7518420235941963</v>
       </c>
       <c r="D5" t="n">
-        <v>0.2964457594820074</v>
+        <v>0.2964457579519918</v>
       </c>
       <c r="E5" t="n">
-        <v>0.3141584338671355</v>
+        <v>0.3141584322457013</v>
       </c>
       <c r="F5" t="n">
-        <v>1.000000030774854</v>
+        <v>1.000000025613655</v>
       </c>
     </row>
     <row r="6">
@@ -1223,19 +1223,19 @@
         <v>20</v>
       </c>
       <c r="B6" t="n">
-        <v>0.3998504343801063</v>
+        <v>0.3998504351121707</v>
       </c>
       <c r="C6" t="n">
-        <v>0.6001495656198937</v>
+        <v>0.6001495648878292</v>
       </c>
       <c r="D6" t="n">
-        <v>0.3349830298320584</v>
+        <v>0.3349830273834287</v>
       </c>
       <c r="E6" t="n">
-        <v>0.3574303462641036</v>
+        <v>0.3574303436513904</v>
       </c>
       <c r="F6" t="n">
-        <v>1.000000036399592</v>
+        <v>1.000000029089879</v>
       </c>
     </row>
     <row r="7">
@@ -1243,19 +1243,19 @@
         <v>25</v>
       </c>
       <c r="B7" t="n">
-        <v>0.6105547035240795</v>
+        <v>0.610554702715483</v>
       </c>
       <c r="C7" t="n">
-        <v>0.3894452964759205</v>
+        <v>0.389445297284517</v>
       </c>
       <c r="D7" t="n">
-        <v>0.3333915278148021</v>
+        <v>0.3333915253763782</v>
       </c>
       <c r="E7" t="n">
-        <v>0.3558479519681307</v>
+        <v>0.3558479493654607</v>
       </c>
       <c r="F7" t="n">
-        <v>1.000000036419796</v>
+        <v>1.000000029105801</v>
       </c>
     </row>
     <row r="8">
@@ -1263,19 +1263,19 @@
         <v>30</v>
       </c>
       <c r="B8" t="n">
-        <v>0.7730355194975116</v>
+        <v>0.7730355183315438</v>
       </c>
       <c r="C8" t="n">
-        <v>0.2269644805024884</v>
+        <v>0.2269644816684561</v>
       </c>
       <c r="D8" t="n">
-        <v>0.2872627801739042</v>
+        <v>0.2872627789471806</v>
       </c>
       <c r="E8" t="n">
-        <v>0.3048470349424793</v>
+        <v>0.3048470336406641</v>
       </c>
       <c r="F8" t="n">
-        <v>1.000000028987476</v>
+        <v>1.000000024717087</v>
       </c>
     </row>
     <row r="9">
@@ -1283,19 +1283,19 @@
         <v>35</v>
       </c>
       <c r="B9" t="n">
-        <v>0.8725975861993882</v>
+        <v>0.8725975871732472</v>
       </c>
       <c r="C9" t="n">
-        <v>0.1274024138006118</v>
+        <v>0.1274024128267529</v>
       </c>
       <c r="D9" t="n">
-        <v>0.2313380617611586</v>
+        <v>0.2313380623658073</v>
       </c>
       <c r="E9" t="n">
-        <v>0.2401119452666387</v>
+        <v>0.2401119458942197</v>
       </c>
       <c r="F9" t="n">
-        <v>1.000000012641499</v>
+        <v>1.000000015255201</v>
       </c>
     </row>
     <row r="10">
@@ -1303,19 +1303,19 @@
         <v>40</v>
       </c>
       <c r="B10" t="n">
-        <v>0.9392430595250765</v>
+        <v>0.9392430576224161</v>
       </c>
       <c r="C10" t="n">
-        <v>0.06075694047492347</v>
+        <v>0.06075694237758389</v>
       </c>
       <c r="D10" t="n">
-        <v>0.173821703313953</v>
+        <v>0.1738217025610129</v>
       </c>
       <c r="E10" t="n">
-        <v>0.1638644462244244</v>
+        <v>0.163864445514616</v>
       </c>
       <c r="F10" t="n">
-        <v>1.000000013240702</v>
+        <v>1.000000008909022</v>
       </c>
     </row>
     <row r="11">
@@ -1323,19 +1323,19 @@
         <v>45</v>
       </c>
       <c r="B11" t="n">
-        <v>0.9713245340057686</v>
+        <v>0.9713245337903351</v>
       </c>
       <c r="C11" t="n">
-        <v>0.02867546599423149</v>
+        <v>0.02867546620966482</v>
       </c>
       <c r="D11" t="n">
-        <v>0.1317422872997296</v>
+        <v>0.1317422872395128</v>
       </c>
       <c r="E11" t="n">
-        <v>0.1024556477243875</v>
+        <v>0.102455647677557</v>
       </c>
       <c r="F11" t="n">
-        <v>1.000000012738686</v>
+        <v>1.000000012281606</v>
       </c>
     </row>
     <row r="12">
@@ -1343,19 +1343,19 @@
         <v>50</v>
       </c>
       <c r="B12" t="n">
-        <v>0.9903352503015272</v>
+        <v>0.9903352484790724</v>
       </c>
       <c r="C12" t="n">
-        <v>0.009664749698472697</v>
+        <v>0.009664751520927606</v>
       </c>
       <c r="D12" t="n">
-        <v>0.09157059767615071</v>
+        <v>0.09157059733580544</v>
       </c>
       <c r="E12" t="n">
-        <v>0.0344409912828303</v>
+        <v>0.03444099115482167</v>
       </c>
       <c r="F12" t="n">
-        <v>1.000000027855146</v>
+        <v>1.000000024138393</v>
       </c>
     </row>
     <row r="13">
@@ -1363,19 +1363,19 @@
         <v>55</v>
       </c>
       <c r="B13" t="n">
-        <v>0.9963286455769149</v>
+        <v>0.9963286414330832</v>
       </c>
       <c r="C13" t="n">
-        <v>0.003671354423085138</v>
+        <v>0.003671358566916749</v>
       </c>
       <c r="D13" t="n">
-        <v>0.04751974177623489</v>
+        <v>0.04751974137949408</v>
       </c>
       <c r="E13" t="n">
-        <v>-0.03741350238665968</v>
+        <v>-0.03741350207429554</v>
       </c>
       <c r="F13" t="n">
-        <v>1.000000040879063</v>
+        <v>1.000000032530095</v>
       </c>
     </row>
     <row r="14">
@@ -1383,19 +1383,19 @@
         <v>60</v>
       </c>
       <c r="B14" t="n">
-        <v>0.9797491418838395</v>
+        <v>0.9797491559709373</v>
       </c>
       <c r="C14" t="n">
-        <v>0.02025085811616045</v>
+        <v>0.0202508440290628</v>
       </c>
       <c r="D14" t="n">
-        <v>0.005167715837012384</v>
+        <v>0.005167715988754432</v>
       </c>
       <c r="E14" t="n">
-        <v>-0.1407624089932488</v>
+        <v>-0.140762413126521</v>
       </c>
       <c r="F14" t="n">
-        <v>1.00000000042167</v>
+        <v>1.000000029785137</v>
       </c>
     </row>
     <row r="15">
@@ -1403,19 +1403,19 @@
         <v>65</v>
       </c>
       <c r="B15" t="n">
-        <v>0.81304262030736</v>
+        <v>0.8130426255251866</v>
       </c>
       <c r="C15" t="n">
-        <v>0.18695737969264</v>
+        <v>0.1869573744748135</v>
       </c>
       <c r="D15" t="n">
-        <v>-0.05869549130762999</v>
+        <v>-0.05869549228597247</v>
       </c>
       <c r="E15" t="n">
-        <v>-0.3854337262534369</v>
+        <v>-0.3854337326778859</v>
       </c>
       <c r="F15" t="n">
-        <v>1.000000000324703</v>
+        <v>1.000000016992806</v>
       </c>
     </row>
     <row r="16">
@@ -1423,19 +1423,19 @@
         <v>70</v>
       </c>
       <c r="B16" t="n">
-        <v>0.1184442191853978</v>
+        <v>0.1184442122109728</v>
       </c>
       <c r="C16" t="n">
-        <v>0.8815557808146022</v>
+        <v>0.8815557877890272</v>
       </c>
       <c r="D16" t="n">
-        <v>-0.04242672488162371</v>
+        <v>-0.04242672565713814</v>
       </c>
       <c r="E16" t="n">
-        <v>-0.3203360100122593</v>
+        <v>-0.3203360158676534</v>
       </c>
       <c r="F16" t="n">
-        <v>1.000000000335592</v>
+        <v>1.000000018614505</v>
       </c>
     </row>
     <row r="17">
@@ -1443,19 +1443,19 @@
         <v>75</v>
       </c>
       <c r="B17" t="n">
-        <v>0.01202997196045735</v>
+        <v>0.01202995707843929</v>
       </c>
       <c r="C17" t="n">
-        <v>0.9879700280395427</v>
+        <v>0.9879700429215608</v>
       </c>
       <c r="D17" t="n">
-        <v>0.02029597067482406</v>
+        <v>0.02029597129380675</v>
       </c>
       <c r="E17" t="n">
-        <v>-0.1071136103585912</v>
+        <v>-0.1071136136253219</v>
       </c>
       <c r="F17" t="n">
-        <v>1.000000000429195</v>
+        <v>1.000000030927007</v>
       </c>
     </row>
     <row r="18">
@@ -1463,19 +1463,19 @@
         <v>80</v>
       </c>
       <c r="B18" t="n">
-        <v>0.003710621116476576</v>
+        <v>0.003710624952946551</v>
       </c>
       <c r="C18" t="n">
-        <v>0.9962893788835234</v>
+        <v>0.9962893750470534</v>
       </c>
       <c r="D18" t="n">
-        <v>0.06054730422378987</v>
+        <v>0.06054730375574053</v>
       </c>
       <c r="E18" t="n">
-        <v>-0.005558441043495448</v>
+        <v>-0.005558441000526985</v>
       </c>
       <c r="F18" t="n">
-        <v>1.000000039816391</v>
+        <v>1.000000032086082</v>
       </c>
     </row>
     <row r="19">
@@ -1483,19 +1483,19 @@
         <v>85</v>
       </c>
       <c r="B19" t="n">
-        <v>0.01462418593750031</v>
+        <v>0.01462418698608564</v>
       </c>
       <c r="C19" t="n">
-        <v>0.9853758140624997</v>
+        <v>0.9853758130139143</v>
       </c>
       <c r="D19" t="n">
-        <v>0.1006007154643659</v>
+        <v>0.1006007152470323</v>
       </c>
       <c r="E19" t="n">
-        <v>0.06549677414685051</v>
+        <v>0.06549677400535406</v>
       </c>
       <c r="F19" t="n">
-        <v>1.00000002450484</v>
+        <v>1.000000022344482</v>
       </c>
     </row>
     <row r="20">
@@ -1503,19 +1503,19 @@
         <v>90</v>
       </c>
       <c r="B20" t="n">
-        <v>0.03612809330644667</v>
+        <v>0.03612809502619335</v>
       </c>
       <c r="C20" t="n">
-        <v>0.9638719066935533</v>
+        <v>0.9638719049738067</v>
       </c>
       <c r="D20" t="n">
-        <v>0.1395918121635073</v>
+        <v>0.1395918116459882</v>
       </c>
       <c r="E20" t="n">
-        <v>0.123842588503428</v>
+        <v>0.1238425880442972</v>
       </c>
       <c r="F20" t="n">
-        <v>1.000000013139668</v>
+        <v>1.000000009432294</v>
       </c>
     </row>
   </sheetData>

</xml_diff>